<commit_message>
First simple static mesh exporter for blender.
</commit_message>
<xml_diff>
--- a/docs/Binary data model.xlsx
+++ b/docs/Binary data model.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="360" windowWidth="28275" windowHeight="13575"/>
   </bookViews>
   <sheets>
-    <sheet name="MeshData" sheetId="1" r:id="rId1"/>
-    <sheet name="PhysicsData" sheetId="2" r:id="rId2"/>
-    <sheet name="Geometry" sheetId="3" r:id="rId3"/>
+    <sheet name="Overview" sheetId="4" r:id="rId1"/>
+    <sheet name="MeshData" sheetId="1" r:id="rId2"/>
+    <sheet name="PhysicsData" sheetId="2" r:id="rId3"/>
+    <sheet name="Geometry" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Mesh Data Definition</t>
   </si>
@@ -42,9 +43,6 @@
     <t>&lt;int&gt; Stream</t>
   </si>
   <si>
-    <t>&lt;int&gt; Mesh Data Version (Currently 1)</t>
-  </si>
-  <si>
     <t>&lt;int&gt; Number of submeshes</t>
   </si>
   <si>
@@ -54,15 +52,9 @@
     <t>&lt;int&gt; Number of streams</t>
   </si>
   <si>
-    <t>&lt;int&gt; Stream size in bytes</t>
-  </si>
-  <si>
     <t>&lt;blob&gt; Vertex data, according to the  vertex declaration and the number of vertices</t>
   </si>
   <si>
-    <t>&lt;int&gt; Number of LODs (min 1)</t>
-  </si>
-  <si>
     <t>&lt;int&gt; Number of indices</t>
   </si>
   <si>
@@ -75,9 +67,6 @@
     <t>&lt;int&gt; Material Index</t>
   </si>
   <si>
-    <t>&lt;int&gt; Physics Data Version (Currently 1)</t>
-  </si>
-  <si>
     <t>&lt;int&gt; Number of physical elements</t>
   </si>
   <si>
@@ -135,24 +124,6 @@
     <t>Physics Data Definition</t>
   </si>
   <si>
-    <t>&lt;geometry&gt;</t>
-  </si>
-  <si>
-    <t>&lt;material name="MaterialName" src="${Materials}/MyMaterial.xml" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;mesh name="Mesh" src=${Meshes/MyMesh.xml" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/geometry&gt;</t>
-  </si>
-  <si>
-    <t>Physics is not handled at this location. This geometry definition is for the valkyrie.graphics.scene not the physics system</t>
-  </si>
-  <si>
-    <t>&lt;string&gt; Name of the element</t>
-  </si>
-  <si>
     <t>Strings are encoded as follows:</t>
   </si>
   <si>
@@ -162,7 +133,31 @@
     <t>&lt;int&gt; Number of characters (including null terminator)</t>
   </si>
   <si>
-    <t>&lt;string&gt; Name of the submesh</t>
+    <t>&lt;int&gt; LOD</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Number of materials</t>
+  </si>
+  <si>
+    <t>&lt;string&gt; Name of material</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Version (Currently = 1)</t>
+  </si>
+  <si>
+    <t>&lt;string&gt; Name of entry</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Number of entries</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Byte offset from beginning of the file</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Type of entry (Mesh, CollisionShape, Skeleton, GeometryData, Animation)</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Size in bytes of the entrie</t>
   </si>
 </sst>
 </file>
@@ -207,9 +202,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -511,10 +507,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T23"/>
+  <dimension ref="B3:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:T22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +570,7 @@
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -544,112 +588,110 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" t="s">
-        <v>47</v>
-      </c>
+      <c r="N11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P12" t="s">
-        <v>46</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="P13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>12</v>
+      <c r="D18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -657,12 +699,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R26"/>
+  <dimension ref="A2:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:R12"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,15 +716,15 @@
     <col min="13" max="13" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -691,129 +733,126 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -821,45 +860,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C9"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="5.7109375" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More on exporting (from blender) static meshes and importing (in valkyrie engine)
</commit_message>
<xml_diff>
--- a/docs/Binary data model.xlsx
+++ b/docs/Binary data model.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="360" windowWidth="28275" windowHeight="13575"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="28275" windowHeight="13515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Mesh Data Definition</t>
   </si>
@@ -118,9 +118,6 @@
     <t>File Extension: VKP</t>
   </si>
   <si>
-    <t>File Extension: VKM</t>
-  </si>
-  <si>
     <t>Physics Data Definition</t>
   </si>
   <si>
@@ -158,6 +155,15 @@
   </si>
   <si>
     <t>&lt;int&gt; Size in bytes of the entrie</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; Magic Number ('MESH')</t>
+  </si>
+  <si>
+    <t>Static Mesh Data format</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; stream stride</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C8"/>
+  <dimension ref="B4:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,34 +524,53 @@
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -555,10 +580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T22"/>
+  <dimension ref="B4:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,12 +593,7 @@
     <col min="4" max="4" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -586,42 +606,42 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -630,36 +650,36 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>4</v>
       </c>
       <c r="P13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>7</v>
       </c>
@@ -676,21 +696,26 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -724,7 +749,7 @@
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>

<commit_message>
Added loader for collision shapes and for rigid body state.
</commit_message>
<xml_diff>
--- a/docs/Binary data model.xlsx
+++ b/docs/Binary data model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="420" windowWidth="28275" windowHeight="13515" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="28275" windowHeight="13515" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>Mesh Data Definition</t>
   </si>
@@ -88,21 +88,6 @@
     <t>&lt;int&gt; Shape type (Sphere, Cylinder, Capsule, Box, TriMesh)</t>
   </si>
   <si>
-    <t>Sphere:</t>
-  </si>
-  <si>
-    <t>Cylinder:</t>
-  </si>
-  <si>
-    <t>Capsule:</t>
-  </si>
-  <si>
-    <t>Box:</t>
-  </si>
-  <si>
-    <t>TriMesh:</t>
-  </si>
-  <si>
     <t>&lt;float3&gt; Vertices</t>
   </si>
   <si>
@@ -218,6 +203,24 @@
   </si>
   <si>
     <t>&lt;string&gt; Material Name</t>
+  </si>
+  <si>
+    <t>&lt;int&gt; axis (0 -&gt; x ; 1 -&gt; y ; 2 -&gt; z)</t>
+  </si>
+  <si>
+    <t>Sphere: 0</t>
+  </si>
+  <si>
+    <t>Cylinder:    X: 1    Y: 2    Z: 3</t>
+  </si>
+  <si>
+    <t>Capsule: X: 4   Y: 5   Z: 6</t>
+  </si>
+  <si>
+    <t>Box: 7</t>
+  </si>
+  <si>
+    <t>TriMesh: 10</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="B4:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +584,7 @@
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -594,37 +597,37 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -662,12 +665,12 @@
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -682,7 +685,7 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -695,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -709,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -720,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="P13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
@@ -750,7 +753,7 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
@@ -775,12 +778,12 @@
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -790,10 +793,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U24"/>
+  <dimension ref="A2:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,13 +810,13 @@
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -829,7 +832,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -839,7 +842,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -860,7 +863,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -876,72 +879,104 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>18</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>18</v>
+      <c r="E14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>19</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>26</v>
+      <c r="F16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
-        <v>19</v>
+      <c r="E18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>27</v>
+      <c r="F20" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G22" t="s">
-        <v>28</v>
+      <c r="E22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +1003,7 @@
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -982,87 +1017,87 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added asset loader for new file format. Added asset input/output stream for generic handling of binary files.
</commit_message>
<xml_diff>
--- a/docs/Binary data model.xlsx
+++ b/docs/Binary data model.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="420" windowWidth="28275" windowHeight="13515" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="28275" windowHeight="13515" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
     <sheet name="MeshData" sheetId="1" r:id="rId2"/>
     <sheet name="PhysicsData" sheetId="2" r:id="rId3"/>
     <sheet name="Geometry" sheetId="3" r:id="rId4"/>
+    <sheet name="AssetDataModel" sheetId="5" r:id="rId5"/>
+    <sheet name="Material" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
   <si>
     <t>Mesh Data Definition</t>
   </si>
@@ -221,6 +223,111 @@
   </si>
   <si>
     <t>TriMesh: 10</t>
+  </si>
+  <si>
+    <t>Magic Number</t>
+  </si>
+  <si>
+    <t>"VALASSET"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;8 byte&gt; </t>
+  </si>
+  <si>
+    <t>&lt;1 byte&gt;</t>
+  </si>
+  <si>
+    <t>Number of entries</t>
+  </si>
+  <si>
+    <t>&lt;8 byte&gt; TYPE_ID</t>
+  </si>
+  <si>
+    <t>&lt;32 byte&gt; Name</t>
+  </si>
+  <si>
+    <t>&lt;4 byte&gt; Offset</t>
+  </si>
+  <si>
+    <t>Shader graph</t>
+  </si>
+  <si>
+    <t>vkShaderGraphAssetLoader</t>
+  </si>
+  <si>
+    <t>CLASS:</t>
+  </si>
+  <si>
+    <t>Num Nodes</t>
+  </si>
+  <si>
+    <t>&lt;uint16&gt;</t>
+  </si>
+  <si>
+    <t>&lt;uint32&gt;</t>
+  </si>
+  <si>
+    <t>Local IDX</t>
+  </si>
+  <si>
+    <t>&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>Node Class Name</t>
+  </si>
+  <si>
+    <t>Num Inputs</t>
+  </si>
+  <si>
+    <t>&lt;vec2&gt;</t>
+  </si>
+  <si>
+    <t>Location within Editor</t>
+  </si>
+  <si>
+    <t>&lt;uint8&gt;</t>
+  </si>
+  <si>
+    <t>Input IDX</t>
+  </si>
+  <si>
+    <t>Input type (0 = Const, 1=ExternalNode)</t>
+  </si>
+  <si>
+    <t>&lt;float&gt;</t>
+  </si>
+  <si>
+    <t>Const float</t>
+  </si>
+  <si>
+    <t>Local OutputNode IDX</t>
+  </si>
+  <si>
+    <t>Local Node Input IDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;uint8&gt; </t>
+  </si>
+  <si>
+    <t>Output IDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;uint16&gt; </t>
+  </si>
+  <si>
+    <t>Num Graph Inputs</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Num Graph Attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;string&gt; </t>
+  </si>
+  <si>
+    <t>&lt;types&gt;</t>
   </si>
 </sst>
 </file>
@@ -795,7 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1103,4 +1210,226 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>